<commit_message>
Gen 3. Out of service.
</commit_message>
<xml_diff>
--- a/data/CS5/case9/case9_2035.xlsx
+++ b/data/CS5/case9/case9_2035.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS5\case9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372155DD-09E4-4818-A6CA-D4D66E5B34FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14666C33-595A-4C67-BED2-4581A462E249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31575" yWindow="-11220" windowWidth="17280" windowHeight="9960" tabRatio="722" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-14400" windowWidth="38640" windowHeight="21120" tabRatio="722" firstSheet="71" activeTab="82" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -4400,7 +4400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -31062,7 +31062,7 @@
   <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U43" sqref="U43"/>
+      <selection activeCell="B4" sqref="B4:Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31303,76 +31303,76 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
@@ -65669,8 +65669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49630D89-783A-49F7-9E51-4F1FD5546230}">
   <dimension ref="A1:Y10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -65911,76 +65911,76 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">

</xml_diff>